<commit_message>
final push before conversion to xml configurations
</commit_message>
<xml_diff>
--- a/src/test/resources/interstellar.xlsx
+++ b/src/test/resources/interstellar.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Kapeshi.Kongolo\My Documents\GitHub\InterstellarTransportSystem\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Kapeshi.Kongolo\My Documents\GitHub\planetstransportsystem\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planet Names" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>Planet Node</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>H</t>
   </si>
   <si>
     <t>Earth</t>
@@ -181,8 +178,36 @@
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -459,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -480,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -488,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -496,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -504,7 +529,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -512,7 +537,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -526,7 +551,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,16 +563,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -600,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4">
         <v>2.44</v>
@@ -611,7 +636,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -629,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,16 +668,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -711,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4">
         <v>0.2</v>
@@ -724,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>

</xml_diff>